<commit_message>
Scrape, preprocess for Aljazeeraenglsih
</commit_message>
<xml_diff>
--- a/social_media_scraper/Final_Output/social_media_posts.xlsx
+++ b/social_media_scraper/Final_Output/social_media_posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Social Media Analytics Dashboard\social_media_scraper\Final_Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1A1C1D-4849-4F0C-81B2-28B17AF1E87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE02AAE-C423-4488-BCF1-DE333F4E3DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3303,7 +3303,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -3359,7 +3359,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3665,10 +3665,14 @@
   <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3755,7 +3759,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N2" t="s">
         <v>21</v>
@@ -3799,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N3" t="s">
         <v>21</v>
@@ -3840,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N4" t="s">
         <v>21</v>
@@ -3887,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N5" t="s">
         <v>21</v>
@@ -3934,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N6" t="s">
         <v>21</v>
@@ -3981,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N7" t="s">
         <v>21</v>
@@ -4028,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N8" t="s">
         <v>40</v>
@@ -4075,7 +4079,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N9" t="s">
         <v>21</v>
@@ -4122,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N10" t="s">
         <v>21</v>
@@ -4169,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N11" t="s">
         <v>40</v>
@@ -4216,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N12" t="s">
         <v>21</v>
@@ -4263,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N13" t="s">
         <v>21</v>
@@ -4310,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N14" t="s">
         <v>21</v>
@@ -4357,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N15" t="s">
         <v>40</v>
@@ -4404,7 +4408,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N16" t="s">
         <v>21</v>
@@ -4451,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>14000000</v>
       </c>
       <c r="N17" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Improve Followers Per Platform, Engagement Metrics, Most Active Times and Traffic indicators based on data scraped
</commit_message>
<xml_diff>
--- a/social_media_scraper/Final_Output/social_media_posts.xlsx
+++ b/social_media_scraper/Final_Output/social_media_posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Social Media Analytics Dashboard\social_media_scraper\Final_Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE02AAE-C423-4488-BCF1-DE333F4E3DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DA07B1-6FC8-449F-955E-148CD9A40873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3664,14 +3664,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="1" max="16" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>